<commit_message>
creat l'apartat per les data quality
</commit_message>
<xml_diff>
--- a/temporal/ExempleCameresBerta.xlsx
+++ b/temporal/ExempleCameresBerta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BertaPhotosDatastreams" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="92">
   <si>
     <t>@iot.selfLink L</t>
   </si>
@@ -111,9 +111,6 @@
     <t>{"resolution" : "24 megapixels", "fieldOfView": "55 degrees", "detectionAngle": "45 degrees"}</t>
   </si>
   <si>
-    <t>Optics in BROWNING DARK OPS PRO X 1080</t>
-  </si>
-  <si>
     <t>properties O</t>
   </si>
   <si>
@@ -286,6 +283,27 @@
   </si>
   <si>
     <t>PHOTOS (URL)</t>
+  </si>
+  <si>
+    <t>https://frost.iotlab.com/sensorthings2/v1.1/Sensors(42)</t>
+  </si>
+  <si>
+    <t>https://frost.iotlab.com/sensorthings2/v1.1/Sensors(43)</t>
+  </si>
+  <si>
+    <t>https://frost.iotlab.com/sensorthings2/v1.1/Sensors(44)</t>
+  </si>
+  <si>
+    <t>Optics1</t>
+  </si>
+  <si>
+    <t>Optics2</t>
+  </si>
+  <si>
+    <t>Optics3</t>
+  </si>
+  <si>
+    <t>Optics4</t>
   </si>
 </sst>
 </file>
@@ -363,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -381,6 +399,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -664,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -882,13 +903,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F3"/>
+  <dimension ref="A2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -911,7 +936,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="108" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="2">
@@ -927,10 +952,76 @@
         <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>27</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="2">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -959,10 +1050,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -970,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2">
         <v>41</v>
@@ -982,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1005,15 +1096,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1022,13 +1113,13 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1036,19 +1127,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>1393287</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1056,19 +1147,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4">
         <v>1393288</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1076,19 +1167,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2">
         <v>1393289</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1096,19 +1187,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4">
         <v>1393290</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1116,19 +1207,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2">
         <v>1393291</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1136,19 +1227,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4">
         <v>1393292</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1156,19 +1247,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2">
         <v>1393293</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1176,19 +1267,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="4">
         <v>1393294</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1196,19 +1287,19 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2">
         <v>1393297</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1216,19 +1307,19 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="4">
         <v>1393299</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1236,19 +1327,19 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2">
         <v>1393300</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1256,19 +1347,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="4">
         <v>1393304</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1276,19 +1367,19 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2">
         <v>1393305</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1296,19 +1387,19 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4">
         <v>1393306</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1316,19 +1407,19 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2">
         <v>1393307</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1336,19 +1427,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="4">
         <v>1393309</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="F19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1356,19 +1447,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2">
         <v>1393310</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1376,19 +1467,19 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4">
         <v>1393311</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1396,19 +1487,19 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2">
         <v>1393313</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="108" x14ac:dyDescent="0.25">
@@ -1416,19 +1507,19 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="4">
         <v>1393314</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>